<commit_message>
Project 4 done , only Create and read added
</commit_message>
<xml_diff>
--- a/Connected Office Web Application/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application/Connected Office Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evoPRo\Desktop\4rde jaar bscIT2022\Semester 2\CMPG323\Projects\Project 4\CMPG323-Project-4-30415284\Connected Office Web Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212E8457-85EA-4AAE-80A2-EFE3F8450632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE44BDED-B597-49B5-85AE-C4D37B386034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19200" yWindow="4245" windowWidth="18900" windowHeight="11505" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1161,7 +1161,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>0</v>
@@ -1178,7 +1178,7 @@
         <v>58</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>0</v>
@@ -1195,7 +1195,7 @@
         <v>59</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>0</v>
@@ -1212,7 +1212,7 @@
         <v>60</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>0</v>
@@ -1229,7 +1229,7 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
@@ -1246,7 +1246,7 @@
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>0</v>
@@ -1263,7 +1263,7 @@
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>0</v>
@@ -1280,7 +1280,7 @@
         <v>64</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>0</v>
@@ -1297,7 +1297,7 @@
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>0</v>
@@ -1314,7 +1314,7 @@
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>0</v>
@@ -1331,7 +1331,7 @@
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>0</v>
@@ -1348,7 +1348,7 @@
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>0</v>
@@ -1365,7 +1365,7 @@
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>0</v>
@@ -1382,7 +1382,7 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="b">
         <v>0</v>

</xml_diff>